<commit_message>
Updated visuals and added terminology
</commit_message>
<xml_diff>
--- a/Automotive.xlsx
+++ b/Automotive.xlsx
@@ -9,6 +9,7 @@
     <sheet state="visible" name="Africa" sheetId="4" r:id="rId7"/>
     <sheet state="visible" name="Asia" sheetId="5" r:id="rId8"/>
     <sheet state="visible" name="Australia" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="Terminology" sheetId="7" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="65">
   <si>
     <t>Company Name</t>
   </si>
@@ -130,6 +131,87 @@
   </si>
   <si>
     <t>Notes / Comments</t>
+  </si>
+  <si>
+    <t>The official registered name of the automotive company.</t>
+  </si>
+  <si>
+    <t>The company's main website, providing details on services, inventory, and contact information.</t>
+  </si>
+  <si>
+    <t>The city and country where the company's head office is based.</t>
+  </si>
+  <si>
+    <t>The complete physical address of the company’s main office or facility.</t>
+  </si>
+  <si>
+    <t>Geographic regions or countries where the company operates or provides services.</t>
+  </si>
+  <si>
+    <t>Strategic markets or regions where the company has a significant footprint.</t>
+  </si>
+  <si>
+    <t>Total number of years the company has been active in the automotive sector.</t>
+  </si>
+  <si>
+    <t>A concise overview of the company’s background, mission, and market focus.</t>
+  </si>
+  <si>
+    <t>Languages spoken by staff for communication and customer service.</t>
+  </si>
+  <si>
+    <t>URL of the company’s LinkedIn profile for corporate updates and networking.</t>
+  </si>
+  <si>
+    <t>Nature of the company’s business (e.g., Dealer, Restorer, Importer, OEM, Customizer).</t>
+  </si>
+  <si>
+    <t>Primary services the company provides (e.g., vehicle sales, servicing, modification, storage).</t>
+  </si>
+  <si>
+    <t>Categories of vehicles the company focuses on (e.g., classic cars, luxury SUVs, hypercars).</t>
+  </si>
+  <si>
+    <t>Specific vehicle body types the company is experienced with (e.g., coupé, convertible, sedan).</t>
+  </si>
+  <si>
+    <t>Official relationships with automotive manufacturers (e.g., Ferrari, Mercedes-Benz).</t>
+  </si>
+  <si>
+    <t>Brands the company frequently works with or holds deep expertise in.</t>
+  </si>
+  <si>
+    <t>Types of vehicles typically in stock (e.g., luxury vehicles, collector cars, electric vehicles).</t>
+  </si>
+  <si>
+    <t>Industry certifications or memberships (e.g., ISO, ASE, manufacturer-authorized programs).</t>
+  </si>
+  <si>
+    <t>Description of physical facilities such as showrooms, service bays, restoration shops, etc.</t>
+  </si>
+  <si>
+    <t>Automotive services performed internally without third-party outsourcing (e.g., detailing, engine rebuilds).</t>
+  </si>
+  <si>
+    <t>Experience converting or certifying vehicles to meet specific regional compliance and safety standards.</t>
+  </si>
+  <si>
+    <t>Name of the main point of contact within the company.</t>
+  </si>
+  <si>
+    <t>Job title or position of the primary contact person.</t>
+  </si>
+  <si>
+    <t>Direct email for the primary contact.</t>
+  </si>
+  <si>
+    <t>Phone number for reaching the primary contact.</t>
+  </si>
+  <si>
+    <t>Professional social media link (e.g., LinkedIn profile) of the contact person.</t>
+  </si>
+  <si>
+    <t>Any additional information, observations, or relationship notes.</t>
   </si>
 </sst>
 </file>
@@ -169,16 +251,20 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -208,6 +294,10 @@
 </file>
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -414,6 +504,46 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="13.63"/>
+    <col customWidth="1" min="2" max="2" width="7.38"/>
+    <col customWidth="1" min="3" max="3" width="11.75"/>
+    <col customWidth="1" min="4" max="4" width="11.13"/>
+    <col customWidth="1" min="5" max="5" width="18.88"/>
+    <col customWidth="1" min="6" max="6" width="21.5"/>
+    <col customWidth="1" min="7" max="7" width="15.75"/>
+    <col customWidth="1" min="8" max="8" width="18.0"/>
+    <col customWidth="1" min="9" max="9" width="16.25"/>
+    <col customWidth="1" min="10" max="10" width="21.5"/>
+    <col customWidth="1" min="11" max="11" width="10.38"/>
+    <col customWidth="1" min="12" max="12" width="12.88"/>
+    <col customWidth="1" min="13" max="13" width="18.5"/>
+    <col customWidth="1" min="14" max="14" width="22.5"/>
+    <col customWidth="1" min="15" max="15" width="21.13"/>
+    <col customWidth="1" min="16" max="16" width="15.5"/>
+    <col customWidth="1" min="17" max="17" width="21.75"/>
+    <col customWidth="1" min="18" max="18" width="27.88"/>
+    <col customWidth="1" min="19" max="19" width="21.63"/>
+    <col customWidth="1" min="20" max="20" width="28.75"/>
+    <col customWidth="1" min="21" max="21" width="18.0"/>
+    <col customWidth="1" min="22" max="22" width="21.5"/>
+    <col customWidth="1" min="23" max="23" width="14.63"/>
+    <col customWidth="1" min="24" max="24" width="13.5"/>
+    <col customWidth="1" min="25" max="25" width="14.5"/>
+    <col customWidth="1" min="26" max="26" width="15.13"/>
+    <col customWidth="1" min="27" max="27" width="15.0"/>
+    <col customWidth="1" min="28" max="28" width="14.63"/>
+    <col customWidth="1" min="29" max="29" width="13.5"/>
+    <col customWidth="1" min="30" max="30" width="14.5"/>
+    <col customWidth="1" min="31" max="31" width="15.13"/>
+    <col customWidth="1" min="32" max="32" width="15.0"/>
+    <col customWidth="1" min="33" max="33" width="14.63"/>
+    <col customWidth="1" min="34" max="34" width="13.5"/>
+    <col customWidth="1" min="35" max="35" width="14.5"/>
+    <col customWidth="1" min="36" max="36" width="15.13"/>
+    <col customWidth="1" min="37" max="37" width="15.0"/>
+    <col customWidth="1" min="38" max="38" width="15.63"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -545,6 +675,46 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="13.63"/>
+    <col customWidth="1" min="2" max="2" width="7.38"/>
+    <col customWidth="1" min="3" max="3" width="11.75"/>
+    <col customWidth="1" min="4" max="4" width="11.13"/>
+    <col customWidth="1" min="5" max="5" width="18.88"/>
+    <col customWidth="1" min="6" max="6" width="21.5"/>
+    <col customWidth="1" min="7" max="7" width="15.75"/>
+    <col customWidth="1" min="8" max="8" width="18.0"/>
+    <col customWidth="1" min="9" max="9" width="16.25"/>
+    <col customWidth="1" min="10" max="10" width="21.5"/>
+    <col customWidth="1" min="11" max="11" width="10.38"/>
+    <col customWidth="1" min="12" max="12" width="12.88"/>
+    <col customWidth="1" min="13" max="13" width="18.5"/>
+    <col customWidth="1" min="14" max="14" width="22.5"/>
+    <col customWidth="1" min="15" max="15" width="21.13"/>
+    <col customWidth="1" min="16" max="16" width="15.5"/>
+    <col customWidth="1" min="17" max="17" width="21.75"/>
+    <col customWidth="1" min="18" max="18" width="27.88"/>
+    <col customWidth="1" min="19" max="19" width="21.63"/>
+    <col customWidth="1" min="20" max="20" width="28.75"/>
+    <col customWidth="1" min="21" max="21" width="18.0"/>
+    <col customWidth="1" min="22" max="22" width="21.5"/>
+    <col customWidth="1" min="23" max="23" width="14.63"/>
+    <col customWidth="1" min="24" max="24" width="13.5"/>
+    <col customWidth="1" min="25" max="25" width="14.5"/>
+    <col customWidth="1" min="26" max="26" width="15.13"/>
+    <col customWidth="1" min="27" max="27" width="15.0"/>
+    <col customWidth="1" min="28" max="28" width="14.63"/>
+    <col customWidth="1" min="29" max="29" width="13.5"/>
+    <col customWidth="1" min="30" max="30" width="14.5"/>
+    <col customWidth="1" min="31" max="31" width="15.13"/>
+    <col customWidth="1" min="32" max="32" width="15.0"/>
+    <col customWidth="1" min="33" max="33" width="14.63"/>
+    <col customWidth="1" min="34" max="34" width="13.5"/>
+    <col customWidth="1" min="35" max="35" width="14.5"/>
+    <col customWidth="1" min="36" max="36" width="15.13"/>
+    <col customWidth="1" min="37" max="37" width="15.0"/>
+    <col customWidth="1" min="38" max="38" width="15.63"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -676,6 +846,46 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="13.63"/>
+    <col customWidth="1" min="2" max="2" width="7.38"/>
+    <col customWidth="1" min="3" max="3" width="11.75"/>
+    <col customWidth="1" min="4" max="4" width="11.13"/>
+    <col customWidth="1" min="5" max="5" width="18.88"/>
+    <col customWidth="1" min="6" max="6" width="21.5"/>
+    <col customWidth="1" min="7" max="7" width="15.75"/>
+    <col customWidth="1" min="8" max="8" width="18.0"/>
+    <col customWidth="1" min="9" max="9" width="16.25"/>
+    <col customWidth="1" min="10" max="10" width="21.5"/>
+    <col customWidth="1" min="11" max="11" width="10.38"/>
+    <col customWidth="1" min="12" max="12" width="12.88"/>
+    <col customWidth="1" min="13" max="13" width="18.5"/>
+    <col customWidth="1" min="14" max="14" width="22.5"/>
+    <col customWidth="1" min="15" max="15" width="21.13"/>
+    <col customWidth="1" min="16" max="16" width="15.5"/>
+    <col customWidth="1" min="17" max="17" width="21.75"/>
+    <col customWidth="1" min="18" max="18" width="27.88"/>
+    <col customWidth="1" min="19" max="19" width="21.63"/>
+    <col customWidth="1" min="20" max="20" width="28.75"/>
+    <col customWidth="1" min="21" max="21" width="18.0"/>
+    <col customWidth="1" min="22" max="22" width="21.5"/>
+    <col customWidth="1" min="23" max="23" width="14.63"/>
+    <col customWidth="1" min="24" max="24" width="13.5"/>
+    <col customWidth="1" min="25" max="25" width="14.5"/>
+    <col customWidth="1" min="26" max="26" width="15.13"/>
+    <col customWidth="1" min="27" max="27" width="15.0"/>
+    <col customWidth="1" min="28" max="28" width="14.63"/>
+    <col customWidth="1" min="29" max="29" width="13.5"/>
+    <col customWidth="1" min="30" max="30" width="14.5"/>
+    <col customWidth="1" min="31" max="31" width="15.13"/>
+    <col customWidth="1" min="32" max="32" width="15.0"/>
+    <col customWidth="1" min="33" max="33" width="14.63"/>
+    <col customWidth="1" min="34" max="34" width="13.5"/>
+    <col customWidth="1" min="35" max="35" width="14.5"/>
+    <col customWidth="1" min="36" max="36" width="15.13"/>
+    <col customWidth="1" min="37" max="37" width="15.0"/>
+    <col customWidth="1" min="38" max="38" width="15.63"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -807,6 +1017,46 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="13.63"/>
+    <col customWidth="1" min="2" max="2" width="7.38"/>
+    <col customWidth="1" min="3" max="3" width="11.75"/>
+    <col customWidth="1" min="4" max="4" width="11.13"/>
+    <col customWidth="1" min="5" max="5" width="18.88"/>
+    <col customWidth="1" min="6" max="6" width="21.5"/>
+    <col customWidth="1" min="7" max="7" width="15.75"/>
+    <col customWidth="1" min="8" max="8" width="18.0"/>
+    <col customWidth="1" min="9" max="9" width="16.25"/>
+    <col customWidth="1" min="10" max="10" width="21.5"/>
+    <col customWidth="1" min="11" max="11" width="10.38"/>
+    <col customWidth="1" min="12" max="12" width="12.88"/>
+    <col customWidth="1" min="13" max="13" width="18.5"/>
+    <col customWidth="1" min="14" max="14" width="22.5"/>
+    <col customWidth="1" min="15" max="15" width="21.13"/>
+    <col customWidth="1" min="16" max="16" width="15.5"/>
+    <col customWidth="1" min="17" max="17" width="21.75"/>
+    <col customWidth="1" min="18" max="18" width="27.88"/>
+    <col customWidth="1" min="19" max="19" width="21.63"/>
+    <col customWidth="1" min="20" max="20" width="28.75"/>
+    <col customWidth="1" min="21" max="21" width="18.0"/>
+    <col customWidth="1" min="22" max="22" width="21.5"/>
+    <col customWidth="1" min="23" max="23" width="14.63"/>
+    <col customWidth="1" min="24" max="24" width="13.5"/>
+    <col customWidth="1" min="25" max="25" width="14.5"/>
+    <col customWidth="1" min="26" max="26" width="15.13"/>
+    <col customWidth="1" min="27" max="27" width="15.0"/>
+    <col customWidth="1" min="28" max="28" width="14.63"/>
+    <col customWidth="1" min="29" max="29" width="13.5"/>
+    <col customWidth="1" min="30" max="30" width="14.5"/>
+    <col customWidth="1" min="31" max="31" width="15.13"/>
+    <col customWidth="1" min="32" max="32" width="15.0"/>
+    <col customWidth="1" min="33" max="33" width="14.63"/>
+    <col customWidth="1" min="34" max="34" width="13.5"/>
+    <col customWidth="1" min="35" max="35" width="14.5"/>
+    <col customWidth="1" min="36" max="36" width="15.13"/>
+    <col customWidth="1" min="37" max="37" width="15.0"/>
+    <col customWidth="1" min="38" max="38" width="15.63"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -938,6 +1188,46 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="13.63"/>
+    <col customWidth="1" min="2" max="2" width="7.38"/>
+    <col customWidth="1" min="3" max="3" width="11.75"/>
+    <col customWidth="1" min="4" max="4" width="11.13"/>
+    <col customWidth="1" min="5" max="5" width="18.88"/>
+    <col customWidth="1" min="6" max="6" width="21.5"/>
+    <col customWidth="1" min="7" max="7" width="15.75"/>
+    <col customWidth="1" min="8" max="8" width="18.0"/>
+    <col customWidth="1" min="9" max="9" width="16.25"/>
+    <col customWidth="1" min="10" max="10" width="21.5"/>
+    <col customWidth="1" min="11" max="11" width="10.38"/>
+    <col customWidth="1" min="12" max="12" width="12.88"/>
+    <col customWidth="1" min="13" max="13" width="18.5"/>
+    <col customWidth="1" min="14" max="14" width="22.5"/>
+    <col customWidth="1" min="15" max="15" width="21.13"/>
+    <col customWidth="1" min="16" max="16" width="15.5"/>
+    <col customWidth="1" min="17" max="17" width="21.75"/>
+    <col customWidth="1" min="18" max="18" width="27.88"/>
+    <col customWidth="1" min="19" max="19" width="21.63"/>
+    <col customWidth="1" min="20" max="20" width="28.75"/>
+    <col customWidth="1" min="21" max="21" width="18.0"/>
+    <col customWidth="1" min="22" max="22" width="21.5"/>
+    <col customWidth="1" min="23" max="23" width="14.63"/>
+    <col customWidth="1" min="24" max="24" width="13.5"/>
+    <col customWidth="1" min="25" max="25" width="14.5"/>
+    <col customWidth="1" min="26" max="26" width="15.13"/>
+    <col customWidth="1" min="27" max="27" width="15.0"/>
+    <col customWidth="1" min="28" max="28" width="14.63"/>
+    <col customWidth="1" min="29" max="29" width="13.5"/>
+    <col customWidth="1" min="30" max="30" width="14.5"/>
+    <col customWidth="1" min="31" max="31" width="15.13"/>
+    <col customWidth="1" min="32" max="32" width="15.0"/>
+    <col customWidth="1" min="33" max="33" width="14.63"/>
+    <col customWidth="1" min="34" max="34" width="13.5"/>
+    <col customWidth="1" min="35" max="35" width="14.5"/>
+    <col customWidth="1" min="36" max="36" width="15.13"/>
+    <col customWidth="1" min="37" max="37" width="15.0"/>
+    <col customWidth="1" min="38" max="38" width="15.63"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -1069,6 +1359,46 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="13.63"/>
+    <col customWidth="1" min="2" max="2" width="7.38"/>
+    <col customWidth="1" min="3" max="3" width="11.75"/>
+    <col customWidth="1" min="4" max="4" width="11.13"/>
+    <col customWidth="1" min="5" max="5" width="18.88"/>
+    <col customWidth="1" min="6" max="6" width="21.5"/>
+    <col customWidth="1" min="7" max="7" width="15.75"/>
+    <col customWidth="1" min="8" max="8" width="18.0"/>
+    <col customWidth="1" min="9" max="9" width="16.25"/>
+    <col customWidth="1" min="10" max="10" width="21.5"/>
+    <col customWidth="1" min="11" max="11" width="10.38"/>
+    <col customWidth="1" min="12" max="12" width="12.88"/>
+    <col customWidth="1" min="13" max="13" width="18.5"/>
+    <col customWidth="1" min="14" max="14" width="22.5"/>
+    <col customWidth="1" min="15" max="15" width="21.13"/>
+    <col customWidth="1" min="16" max="16" width="15.5"/>
+    <col customWidth="1" min="17" max="17" width="21.75"/>
+    <col customWidth="1" min="18" max="18" width="27.88"/>
+    <col customWidth="1" min="19" max="19" width="21.63"/>
+    <col customWidth="1" min="20" max="20" width="28.75"/>
+    <col customWidth="1" min="21" max="21" width="18.0"/>
+    <col customWidth="1" min="22" max="22" width="21.5"/>
+    <col customWidth="1" min="23" max="23" width="14.63"/>
+    <col customWidth="1" min="24" max="24" width="13.5"/>
+    <col customWidth="1" min="25" max="25" width="14.5"/>
+    <col customWidth="1" min="26" max="26" width="15.13"/>
+    <col customWidth="1" min="27" max="27" width="15.0"/>
+    <col customWidth="1" min="28" max="28" width="14.63"/>
+    <col customWidth="1" min="29" max="29" width="13.5"/>
+    <col customWidth="1" min="30" max="30" width="14.5"/>
+    <col customWidth="1" min="31" max="31" width="15.13"/>
+    <col customWidth="1" min="32" max="32" width="15.0"/>
+    <col customWidth="1" min="33" max="33" width="14.63"/>
+    <col customWidth="1" min="34" max="34" width="13.5"/>
+    <col customWidth="1" min="35" max="35" width="14.5"/>
+    <col customWidth="1" min="36" max="36" width="15.13"/>
+    <col customWidth="1" min="37" max="37" width="15.0"/>
+    <col customWidth="1" min="38" max="38" width="15.63"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -1189,4 +1519,3159 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="29.88"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="4"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="4"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="4"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="4"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="4"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="4"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="4"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="4"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="4"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="4"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="4"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="4"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="4"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="4"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="4"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="4"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="4"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="4"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="4"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="4"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="4"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="4"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="4"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="4"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="4"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="4"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="4"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="4"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="4"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="4"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="4"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="4"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="4"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="4"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="4"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="4"/>
+    </row>
+    <row r="65">
+      <c r="A65" s="4"/>
+    </row>
+    <row r="66">
+      <c r="A66" s="4"/>
+    </row>
+    <row r="67">
+      <c r="A67" s="4"/>
+    </row>
+    <row r="68">
+      <c r="A68" s="4"/>
+    </row>
+    <row r="69">
+      <c r="A69" s="4"/>
+    </row>
+    <row r="70">
+      <c r="A70" s="4"/>
+    </row>
+    <row r="71">
+      <c r="A71" s="4"/>
+    </row>
+    <row r="72">
+      <c r="A72" s="4"/>
+    </row>
+    <row r="73">
+      <c r="A73" s="4"/>
+    </row>
+    <row r="74">
+      <c r="A74" s="4"/>
+    </row>
+    <row r="75">
+      <c r="A75" s="4"/>
+    </row>
+    <row r="76">
+      <c r="A76" s="4"/>
+    </row>
+    <row r="77">
+      <c r="A77" s="4"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="4"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="4"/>
+    </row>
+    <row r="80">
+      <c r="A80" s="4"/>
+    </row>
+    <row r="81">
+      <c r="A81" s="4"/>
+    </row>
+    <row r="82">
+      <c r="A82" s="4"/>
+    </row>
+    <row r="83">
+      <c r="A83" s="4"/>
+    </row>
+    <row r="84">
+      <c r="A84" s="4"/>
+    </row>
+    <row r="85">
+      <c r="A85" s="4"/>
+    </row>
+    <row r="86">
+      <c r="A86" s="4"/>
+    </row>
+    <row r="87">
+      <c r="A87" s="4"/>
+    </row>
+    <row r="88">
+      <c r="A88" s="4"/>
+    </row>
+    <row r="89">
+      <c r="A89" s="4"/>
+    </row>
+    <row r="90">
+      <c r="A90" s="4"/>
+    </row>
+    <row r="91">
+      <c r="A91" s="4"/>
+    </row>
+    <row r="92">
+      <c r="A92" s="4"/>
+    </row>
+    <row r="93">
+      <c r="A93" s="4"/>
+    </row>
+    <row r="94">
+      <c r="A94" s="4"/>
+    </row>
+    <row r="95">
+      <c r="A95" s="4"/>
+    </row>
+    <row r="96">
+      <c r="A96" s="4"/>
+    </row>
+    <row r="97">
+      <c r="A97" s="4"/>
+    </row>
+    <row r="98">
+      <c r="A98" s="4"/>
+    </row>
+    <row r="99">
+      <c r="A99" s="4"/>
+    </row>
+    <row r="100">
+      <c r="A100" s="4"/>
+    </row>
+    <row r="101">
+      <c r="A101" s="4"/>
+    </row>
+    <row r="102">
+      <c r="A102" s="4"/>
+    </row>
+    <row r="103">
+      <c r="A103" s="4"/>
+    </row>
+    <row r="104">
+      <c r="A104" s="4"/>
+    </row>
+    <row r="105">
+      <c r="A105" s="4"/>
+    </row>
+    <row r="106">
+      <c r="A106" s="4"/>
+    </row>
+    <row r="107">
+      <c r="A107" s="4"/>
+    </row>
+    <row r="108">
+      <c r="A108" s="4"/>
+    </row>
+    <row r="109">
+      <c r="A109" s="4"/>
+    </row>
+    <row r="110">
+      <c r="A110" s="4"/>
+    </row>
+    <row r="111">
+      <c r="A111" s="4"/>
+    </row>
+    <row r="112">
+      <c r="A112" s="4"/>
+    </row>
+    <row r="113">
+      <c r="A113" s="4"/>
+    </row>
+    <row r="114">
+      <c r="A114" s="4"/>
+    </row>
+    <row r="115">
+      <c r="A115" s="4"/>
+    </row>
+    <row r="116">
+      <c r="A116" s="4"/>
+    </row>
+    <row r="117">
+      <c r="A117" s="4"/>
+    </row>
+    <row r="118">
+      <c r="A118" s="4"/>
+    </row>
+    <row r="119">
+      <c r="A119" s="4"/>
+    </row>
+    <row r="120">
+      <c r="A120" s="4"/>
+    </row>
+    <row r="121">
+      <c r="A121" s="4"/>
+    </row>
+    <row r="122">
+      <c r="A122" s="4"/>
+    </row>
+    <row r="123">
+      <c r="A123" s="4"/>
+    </row>
+    <row r="124">
+      <c r="A124" s="4"/>
+    </row>
+    <row r="125">
+      <c r="A125" s="4"/>
+    </row>
+    <row r="126">
+      <c r="A126" s="4"/>
+    </row>
+    <row r="127">
+      <c r="A127" s="4"/>
+    </row>
+    <row r="128">
+      <c r="A128" s="4"/>
+    </row>
+    <row r="129">
+      <c r="A129" s="4"/>
+    </row>
+    <row r="130">
+      <c r="A130" s="4"/>
+    </row>
+    <row r="131">
+      <c r="A131" s="4"/>
+    </row>
+    <row r="132">
+      <c r="A132" s="4"/>
+    </row>
+    <row r="133">
+      <c r="A133" s="4"/>
+    </row>
+    <row r="134">
+      <c r="A134" s="4"/>
+    </row>
+    <row r="135">
+      <c r="A135" s="4"/>
+    </row>
+    <row r="136">
+      <c r="A136" s="4"/>
+    </row>
+    <row r="137">
+      <c r="A137" s="4"/>
+    </row>
+    <row r="138">
+      <c r="A138" s="4"/>
+    </row>
+    <row r="139">
+      <c r="A139" s="4"/>
+    </row>
+    <row r="140">
+      <c r="A140" s="4"/>
+    </row>
+    <row r="141">
+      <c r="A141" s="4"/>
+    </row>
+    <row r="142">
+      <c r="A142" s="4"/>
+    </row>
+    <row r="143">
+      <c r="A143" s="4"/>
+    </row>
+    <row r="144">
+      <c r="A144" s="4"/>
+    </row>
+    <row r="145">
+      <c r="A145" s="4"/>
+    </row>
+    <row r="146">
+      <c r="A146" s="4"/>
+    </row>
+    <row r="147">
+      <c r="A147" s="4"/>
+    </row>
+    <row r="148">
+      <c r="A148" s="4"/>
+    </row>
+    <row r="149">
+      <c r="A149" s="4"/>
+    </row>
+    <row r="150">
+      <c r="A150" s="4"/>
+    </row>
+    <row r="151">
+      <c r="A151" s="4"/>
+    </row>
+    <row r="152">
+      <c r="A152" s="4"/>
+    </row>
+    <row r="153">
+      <c r="A153" s="4"/>
+    </row>
+    <row r="154">
+      <c r="A154" s="4"/>
+    </row>
+    <row r="155">
+      <c r="A155" s="4"/>
+    </row>
+    <row r="156">
+      <c r="A156" s="4"/>
+    </row>
+    <row r="157">
+      <c r="A157" s="4"/>
+    </row>
+    <row r="158">
+      <c r="A158" s="4"/>
+    </row>
+    <row r="159">
+      <c r="A159" s="4"/>
+    </row>
+    <row r="160">
+      <c r="A160" s="4"/>
+    </row>
+    <row r="161">
+      <c r="A161" s="4"/>
+    </row>
+    <row r="162">
+      <c r="A162" s="4"/>
+    </row>
+    <row r="163">
+      <c r="A163" s="4"/>
+    </row>
+    <row r="164">
+      <c r="A164" s="4"/>
+    </row>
+    <row r="165">
+      <c r="A165" s="4"/>
+    </row>
+    <row r="166">
+      <c r="A166" s="4"/>
+    </row>
+    <row r="167">
+      <c r="A167" s="4"/>
+    </row>
+    <row r="168">
+      <c r="A168" s="4"/>
+    </row>
+    <row r="169">
+      <c r="A169" s="4"/>
+    </row>
+    <row r="170">
+      <c r="A170" s="4"/>
+    </row>
+    <row r="171">
+      <c r="A171" s="4"/>
+    </row>
+    <row r="172">
+      <c r="A172" s="4"/>
+    </row>
+    <row r="173">
+      <c r="A173" s="4"/>
+    </row>
+    <row r="174">
+      <c r="A174" s="4"/>
+    </row>
+    <row r="175">
+      <c r="A175" s="4"/>
+    </row>
+    <row r="176">
+      <c r="A176" s="4"/>
+    </row>
+    <row r="177">
+      <c r="A177" s="4"/>
+    </row>
+    <row r="178">
+      <c r="A178" s="4"/>
+    </row>
+    <row r="179">
+      <c r="A179" s="4"/>
+    </row>
+    <row r="180">
+      <c r="A180" s="4"/>
+    </row>
+    <row r="181">
+      <c r="A181" s="4"/>
+    </row>
+    <row r="182">
+      <c r="A182" s="4"/>
+    </row>
+    <row r="183">
+      <c r="A183" s="4"/>
+    </row>
+    <row r="184">
+      <c r="A184" s="4"/>
+    </row>
+    <row r="185">
+      <c r="A185" s="4"/>
+    </row>
+    <row r="186">
+      <c r="A186" s="4"/>
+    </row>
+    <row r="187">
+      <c r="A187" s="4"/>
+    </row>
+    <row r="188">
+      <c r="A188" s="4"/>
+    </row>
+    <row r="189">
+      <c r="A189" s="4"/>
+    </row>
+    <row r="190">
+      <c r="A190" s="4"/>
+    </row>
+    <row r="191">
+      <c r="A191" s="4"/>
+    </row>
+    <row r="192">
+      <c r="A192" s="4"/>
+    </row>
+    <row r="193">
+      <c r="A193" s="4"/>
+    </row>
+    <row r="194">
+      <c r="A194" s="4"/>
+    </row>
+    <row r="195">
+      <c r="A195" s="4"/>
+    </row>
+    <row r="196">
+      <c r="A196" s="4"/>
+    </row>
+    <row r="197">
+      <c r="A197" s="4"/>
+    </row>
+    <row r="198">
+      <c r="A198" s="4"/>
+    </row>
+    <row r="199">
+      <c r="A199" s="4"/>
+    </row>
+    <row r="200">
+      <c r="A200" s="4"/>
+    </row>
+    <row r="201">
+      <c r="A201" s="4"/>
+    </row>
+    <row r="202">
+      <c r="A202" s="4"/>
+    </row>
+    <row r="203">
+      <c r="A203" s="4"/>
+    </row>
+    <row r="204">
+      <c r="A204" s="4"/>
+    </row>
+    <row r="205">
+      <c r="A205" s="4"/>
+    </row>
+    <row r="206">
+      <c r="A206" s="4"/>
+    </row>
+    <row r="207">
+      <c r="A207" s="4"/>
+    </row>
+    <row r="208">
+      <c r="A208" s="4"/>
+    </row>
+    <row r="209">
+      <c r="A209" s="4"/>
+    </row>
+    <row r="210">
+      <c r="A210" s="4"/>
+    </row>
+    <row r="211">
+      <c r="A211" s="4"/>
+    </row>
+    <row r="212">
+      <c r="A212" s="4"/>
+    </row>
+    <row r="213">
+      <c r="A213" s="4"/>
+    </row>
+    <row r="214">
+      <c r="A214" s="4"/>
+    </row>
+    <row r="215">
+      <c r="A215" s="4"/>
+    </row>
+    <row r="216">
+      <c r="A216" s="4"/>
+    </row>
+    <row r="217">
+      <c r="A217" s="4"/>
+    </row>
+    <row r="218">
+      <c r="A218" s="4"/>
+    </row>
+    <row r="219">
+      <c r="A219" s="4"/>
+    </row>
+    <row r="220">
+      <c r="A220" s="4"/>
+    </row>
+    <row r="221">
+      <c r="A221" s="4"/>
+    </row>
+    <row r="222">
+      <c r="A222" s="4"/>
+    </row>
+    <row r="223">
+      <c r="A223" s="4"/>
+    </row>
+    <row r="224">
+      <c r="A224" s="4"/>
+    </row>
+    <row r="225">
+      <c r="A225" s="4"/>
+    </row>
+    <row r="226">
+      <c r="A226" s="4"/>
+    </row>
+    <row r="227">
+      <c r="A227" s="4"/>
+    </row>
+    <row r="228">
+      <c r="A228" s="4"/>
+    </row>
+    <row r="229">
+      <c r="A229" s="4"/>
+    </row>
+    <row r="230">
+      <c r="A230" s="4"/>
+    </row>
+    <row r="231">
+      <c r="A231" s="4"/>
+    </row>
+    <row r="232">
+      <c r="A232" s="4"/>
+    </row>
+    <row r="233">
+      <c r="A233" s="4"/>
+    </row>
+    <row r="234">
+      <c r="A234" s="4"/>
+    </row>
+    <row r="235">
+      <c r="A235" s="4"/>
+    </row>
+    <row r="236">
+      <c r="A236" s="4"/>
+    </row>
+    <row r="237">
+      <c r="A237" s="4"/>
+    </row>
+    <row r="238">
+      <c r="A238" s="4"/>
+    </row>
+    <row r="239">
+      <c r="A239" s="4"/>
+    </row>
+    <row r="240">
+      <c r="A240" s="4"/>
+    </row>
+    <row r="241">
+      <c r="A241" s="4"/>
+    </row>
+    <row r="242">
+      <c r="A242" s="4"/>
+    </row>
+    <row r="243">
+      <c r="A243" s="4"/>
+    </row>
+    <row r="244">
+      <c r="A244" s="4"/>
+    </row>
+    <row r="245">
+      <c r="A245" s="4"/>
+    </row>
+    <row r="246">
+      <c r="A246" s="4"/>
+    </row>
+    <row r="247">
+      <c r="A247" s="4"/>
+    </row>
+    <row r="248">
+      <c r="A248" s="4"/>
+    </row>
+    <row r="249">
+      <c r="A249" s="4"/>
+    </row>
+    <row r="250">
+      <c r="A250" s="4"/>
+    </row>
+    <row r="251">
+      <c r="A251" s="4"/>
+    </row>
+    <row r="252">
+      <c r="A252" s="4"/>
+    </row>
+    <row r="253">
+      <c r="A253" s="4"/>
+    </row>
+    <row r="254">
+      <c r="A254" s="4"/>
+    </row>
+    <row r="255">
+      <c r="A255" s="4"/>
+    </row>
+    <row r="256">
+      <c r="A256" s="4"/>
+    </row>
+    <row r="257">
+      <c r="A257" s="4"/>
+    </row>
+    <row r="258">
+      <c r="A258" s="4"/>
+    </row>
+    <row r="259">
+      <c r="A259" s="4"/>
+    </row>
+    <row r="260">
+      <c r="A260" s="4"/>
+    </row>
+    <row r="261">
+      <c r="A261" s="4"/>
+    </row>
+    <row r="262">
+      <c r="A262" s="4"/>
+    </row>
+    <row r="263">
+      <c r="A263" s="4"/>
+    </row>
+    <row r="264">
+      <c r="A264" s="4"/>
+    </row>
+    <row r="265">
+      <c r="A265" s="4"/>
+    </row>
+    <row r="266">
+      <c r="A266" s="4"/>
+    </row>
+    <row r="267">
+      <c r="A267" s="4"/>
+    </row>
+    <row r="268">
+      <c r="A268" s="4"/>
+    </row>
+    <row r="269">
+      <c r="A269" s="4"/>
+    </row>
+    <row r="270">
+      <c r="A270" s="4"/>
+    </row>
+    <row r="271">
+      <c r="A271" s="4"/>
+    </row>
+    <row r="272">
+      <c r="A272" s="4"/>
+    </row>
+    <row r="273">
+      <c r="A273" s="4"/>
+    </row>
+    <row r="274">
+      <c r="A274" s="4"/>
+    </row>
+    <row r="275">
+      <c r="A275" s="4"/>
+    </row>
+    <row r="276">
+      <c r="A276" s="4"/>
+    </row>
+    <row r="277">
+      <c r="A277" s="4"/>
+    </row>
+    <row r="278">
+      <c r="A278" s="4"/>
+    </row>
+    <row r="279">
+      <c r="A279" s="4"/>
+    </row>
+    <row r="280">
+      <c r="A280" s="4"/>
+    </row>
+    <row r="281">
+      <c r="A281" s="4"/>
+    </row>
+    <row r="282">
+      <c r="A282" s="4"/>
+    </row>
+    <row r="283">
+      <c r="A283" s="4"/>
+    </row>
+    <row r="284">
+      <c r="A284" s="4"/>
+    </row>
+    <row r="285">
+      <c r="A285" s="4"/>
+    </row>
+    <row r="286">
+      <c r="A286" s="4"/>
+    </row>
+    <row r="287">
+      <c r="A287" s="4"/>
+    </row>
+    <row r="288">
+      <c r="A288" s="4"/>
+    </row>
+    <row r="289">
+      <c r="A289" s="4"/>
+    </row>
+    <row r="290">
+      <c r="A290" s="4"/>
+    </row>
+    <row r="291">
+      <c r="A291" s="4"/>
+    </row>
+    <row r="292">
+      <c r="A292" s="4"/>
+    </row>
+    <row r="293">
+      <c r="A293" s="4"/>
+    </row>
+    <row r="294">
+      <c r="A294" s="4"/>
+    </row>
+    <row r="295">
+      <c r="A295" s="4"/>
+    </row>
+    <row r="296">
+      <c r="A296" s="4"/>
+    </row>
+    <row r="297">
+      <c r="A297" s="4"/>
+    </row>
+    <row r="298">
+      <c r="A298" s="4"/>
+    </row>
+    <row r="299">
+      <c r="A299" s="4"/>
+    </row>
+    <row r="300">
+      <c r="A300" s="4"/>
+    </row>
+    <row r="301">
+      <c r="A301" s="4"/>
+    </row>
+    <row r="302">
+      <c r="A302" s="4"/>
+    </row>
+    <row r="303">
+      <c r="A303" s="4"/>
+    </row>
+    <row r="304">
+      <c r="A304" s="4"/>
+    </row>
+    <row r="305">
+      <c r="A305" s="4"/>
+    </row>
+    <row r="306">
+      <c r="A306" s="4"/>
+    </row>
+    <row r="307">
+      <c r="A307" s="4"/>
+    </row>
+    <row r="308">
+      <c r="A308" s="4"/>
+    </row>
+    <row r="309">
+      <c r="A309" s="4"/>
+    </row>
+    <row r="310">
+      <c r="A310" s="4"/>
+    </row>
+    <row r="311">
+      <c r="A311" s="4"/>
+    </row>
+    <row r="312">
+      <c r="A312" s="4"/>
+    </row>
+    <row r="313">
+      <c r="A313" s="4"/>
+    </row>
+    <row r="314">
+      <c r="A314" s="4"/>
+    </row>
+    <row r="315">
+      <c r="A315" s="4"/>
+    </row>
+    <row r="316">
+      <c r="A316" s="4"/>
+    </row>
+    <row r="317">
+      <c r="A317" s="4"/>
+    </row>
+    <row r="318">
+      <c r="A318" s="4"/>
+    </row>
+    <row r="319">
+      <c r="A319" s="4"/>
+    </row>
+    <row r="320">
+      <c r="A320" s="4"/>
+    </row>
+    <row r="321">
+      <c r="A321" s="4"/>
+    </row>
+    <row r="322">
+      <c r="A322" s="4"/>
+    </row>
+    <row r="323">
+      <c r="A323" s="4"/>
+    </row>
+    <row r="324">
+      <c r="A324" s="4"/>
+    </row>
+    <row r="325">
+      <c r="A325" s="4"/>
+    </row>
+    <row r="326">
+      <c r="A326" s="4"/>
+    </row>
+    <row r="327">
+      <c r="A327" s="4"/>
+    </row>
+    <row r="328">
+      <c r="A328" s="4"/>
+    </row>
+    <row r="329">
+      <c r="A329" s="4"/>
+    </row>
+    <row r="330">
+      <c r="A330" s="4"/>
+    </row>
+    <row r="331">
+      <c r="A331" s="4"/>
+    </row>
+    <row r="332">
+      <c r="A332" s="4"/>
+    </row>
+    <row r="333">
+      <c r="A333" s="4"/>
+    </row>
+    <row r="334">
+      <c r="A334" s="4"/>
+    </row>
+    <row r="335">
+      <c r="A335" s="4"/>
+    </row>
+    <row r="336">
+      <c r="A336" s="4"/>
+    </row>
+    <row r="337">
+      <c r="A337" s="4"/>
+    </row>
+    <row r="338">
+      <c r="A338" s="4"/>
+    </row>
+    <row r="339">
+      <c r="A339" s="4"/>
+    </row>
+    <row r="340">
+      <c r="A340" s="4"/>
+    </row>
+    <row r="341">
+      <c r="A341" s="4"/>
+    </row>
+    <row r="342">
+      <c r="A342" s="4"/>
+    </row>
+    <row r="343">
+      <c r="A343" s="4"/>
+    </row>
+    <row r="344">
+      <c r="A344" s="4"/>
+    </row>
+    <row r="345">
+      <c r="A345" s="4"/>
+    </row>
+    <row r="346">
+      <c r="A346" s="4"/>
+    </row>
+    <row r="347">
+      <c r="A347" s="4"/>
+    </row>
+    <row r="348">
+      <c r="A348" s="4"/>
+    </row>
+    <row r="349">
+      <c r="A349" s="4"/>
+    </row>
+    <row r="350">
+      <c r="A350" s="4"/>
+    </row>
+    <row r="351">
+      <c r="A351" s="4"/>
+    </row>
+    <row r="352">
+      <c r="A352" s="4"/>
+    </row>
+    <row r="353">
+      <c r="A353" s="4"/>
+    </row>
+    <row r="354">
+      <c r="A354" s="4"/>
+    </row>
+    <row r="355">
+      <c r="A355" s="4"/>
+    </row>
+    <row r="356">
+      <c r="A356" s="4"/>
+    </row>
+    <row r="357">
+      <c r="A357" s="4"/>
+    </row>
+    <row r="358">
+      <c r="A358" s="4"/>
+    </row>
+    <row r="359">
+      <c r="A359" s="4"/>
+    </row>
+    <row r="360">
+      <c r="A360" s="4"/>
+    </row>
+    <row r="361">
+      <c r="A361" s="4"/>
+    </row>
+    <row r="362">
+      <c r="A362" s="4"/>
+    </row>
+    <row r="363">
+      <c r="A363" s="4"/>
+    </row>
+    <row r="364">
+      <c r="A364" s="4"/>
+    </row>
+    <row r="365">
+      <c r="A365" s="4"/>
+    </row>
+    <row r="366">
+      <c r="A366" s="4"/>
+    </row>
+    <row r="367">
+      <c r="A367" s="4"/>
+    </row>
+    <row r="368">
+      <c r="A368" s="4"/>
+    </row>
+    <row r="369">
+      <c r="A369" s="4"/>
+    </row>
+    <row r="370">
+      <c r="A370" s="4"/>
+    </row>
+    <row r="371">
+      <c r="A371" s="4"/>
+    </row>
+    <row r="372">
+      <c r="A372" s="4"/>
+    </row>
+    <row r="373">
+      <c r="A373" s="4"/>
+    </row>
+    <row r="374">
+      <c r="A374" s="4"/>
+    </row>
+    <row r="375">
+      <c r="A375" s="4"/>
+    </row>
+    <row r="376">
+      <c r="A376" s="4"/>
+    </row>
+    <row r="377">
+      <c r="A377" s="4"/>
+    </row>
+    <row r="378">
+      <c r="A378" s="4"/>
+    </row>
+    <row r="379">
+      <c r="A379" s="4"/>
+    </row>
+    <row r="380">
+      <c r="A380" s="4"/>
+    </row>
+    <row r="381">
+      <c r="A381" s="4"/>
+    </row>
+    <row r="382">
+      <c r="A382" s="4"/>
+    </row>
+    <row r="383">
+      <c r="A383" s="4"/>
+    </row>
+    <row r="384">
+      <c r="A384" s="4"/>
+    </row>
+    <row r="385">
+      <c r="A385" s="4"/>
+    </row>
+    <row r="386">
+      <c r="A386" s="4"/>
+    </row>
+    <row r="387">
+      <c r="A387" s="4"/>
+    </row>
+    <row r="388">
+      <c r="A388" s="4"/>
+    </row>
+    <row r="389">
+      <c r="A389" s="4"/>
+    </row>
+    <row r="390">
+      <c r="A390" s="4"/>
+    </row>
+    <row r="391">
+      <c r="A391" s="4"/>
+    </row>
+    <row r="392">
+      <c r="A392" s="4"/>
+    </row>
+    <row r="393">
+      <c r="A393" s="4"/>
+    </row>
+    <row r="394">
+      <c r="A394" s="4"/>
+    </row>
+    <row r="395">
+      <c r="A395" s="4"/>
+    </row>
+    <row r="396">
+      <c r="A396" s="4"/>
+    </row>
+    <row r="397">
+      <c r="A397" s="4"/>
+    </row>
+    <row r="398">
+      <c r="A398" s="4"/>
+    </row>
+    <row r="399">
+      <c r="A399" s="4"/>
+    </row>
+    <row r="400">
+      <c r="A400" s="4"/>
+    </row>
+    <row r="401">
+      <c r="A401" s="4"/>
+    </row>
+    <row r="402">
+      <c r="A402" s="4"/>
+    </row>
+    <row r="403">
+      <c r="A403" s="4"/>
+    </row>
+    <row r="404">
+      <c r="A404" s="4"/>
+    </row>
+    <row r="405">
+      <c r="A405" s="4"/>
+    </row>
+    <row r="406">
+      <c r="A406" s="4"/>
+    </row>
+    <row r="407">
+      <c r="A407" s="4"/>
+    </row>
+    <row r="408">
+      <c r="A408" s="4"/>
+    </row>
+    <row r="409">
+      <c r="A409" s="4"/>
+    </row>
+    <row r="410">
+      <c r="A410" s="4"/>
+    </row>
+    <row r="411">
+      <c r="A411" s="4"/>
+    </row>
+    <row r="412">
+      <c r="A412" s="4"/>
+    </row>
+    <row r="413">
+      <c r="A413" s="4"/>
+    </row>
+    <row r="414">
+      <c r="A414" s="4"/>
+    </row>
+    <row r="415">
+      <c r="A415" s="4"/>
+    </row>
+    <row r="416">
+      <c r="A416" s="4"/>
+    </row>
+    <row r="417">
+      <c r="A417" s="4"/>
+    </row>
+    <row r="418">
+      <c r="A418" s="4"/>
+    </row>
+    <row r="419">
+      <c r="A419" s="4"/>
+    </row>
+    <row r="420">
+      <c r="A420" s="4"/>
+    </row>
+    <row r="421">
+      <c r="A421" s="4"/>
+    </row>
+    <row r="422">
+      <c r="A422" s="4"/>
+    </row>
+    <row r="423">
+      <c r="A423" s="4"/>
+    </row>
+    <row r="424">
+      <c r="A424" s="4"/>
+    </row>
+    <row r="425">
+      <c r="A425" s="4"/>
+    </row>
+    <row r="426">
+      <c r="A426" s="4"/>
+    </row>
+    <row r="427">
+      <c r="A427" s="4"/>
+    </row>
+    <row r="428">
+      <c r="A428" s="4"/>
+    </row>
+    <row r="429">
+      <c r="A429" s="4"/>
+    </row>
+    <row r="430">
+      <c r="A430" s="4"/>
+    </row>
+    <row r="431">
+      <c r="A431" s="4"/>
+    </row>
+    <row r="432">
+      <c r="A432" s="4"/>
+    </row>
+    <row r="433">
+      <c r="A433" s="4"/>
+    </row>
+    <row r="434">
+      <c r="A434" s="4"/>
+    </row>
+    <row r="435">
+      <c r="A435" s="4"/>
+    </row>
+    <row r="436">
+      <c r="A436" s="4"/>
+    </row>
+    <row r="437">
+      <c r="A437" s="4"/>
+    </row>
+    <row r="438">
+      <c r="A438" s="4"/>
+    </row>
+    <row r="439">
+      <c r="A439" s="4"/>
+    </row>
+    <row r="440">
+      <c r="A440" s="4"/>
+    </row>
+    <row r="441">
+      <c r="A441" s="4"/>
+    </row>
+    <row r="442">
+      <c r="A442" s="4"/>
+    </row>
+    <row r="443">
+      <c r="A443" s="4"/>
+    </row>
+    <row r="444">
+      <c r="A444" s="4"/>
+    </row>
+    <row r="445">
+      <c r="A445" s="4"/>
+    </row>
+    <row r="446">
+      <c r="A446" s="4"/>
+    </row>
+    <row r="447">
+      <c r="A447" s="4"/>
+    </row>
+    <row r="448">
+      <c r="A448" s="4"/>
+    </row>
+    <row r="449">
+      <c r="A449" s="4"/>
+    </row>
+    <row r="450">
+      <c r="A450" s="4"/>
+    </row>
+    <row r="451">
+      <c r="A451" s="4"/>
+    </row>
+    <row r="452">
+      <c r="A452" s="4"/>
+    </row>
+    <row r="453">
+      <c r="A453" s="4"/>
+    </row>
+    <row r="454">
+      <c r="A454" s="4"/>
+    </row>
+    <row r="455">
+      <c r="A455" s="4"/>
+    </row>
+    <row r="456">
+      <c r="A456" s="4"/>
+    </row>
+    <row r="457">
+      <c r="A457" s="4"/>
+    </row>
+    <row r="458">
+      <c r="A458" s="4"/>
+    </row>
+    <row r="459">
+      <c r="A459" s="4"/>
+    </row>
+    <row r="460">
+      <c r="A460" s="4"/>
+    </row>
+    <row r="461">
+      <c r="A461" s="4"/>
+    </row>
+    <row r="462">
+      <c r="A462" s="4"/>
+    </row>
+    <row r="463">
+      <c r="A463" s="4"/>
+    </row>
+    <row r="464">
+      <c r="A464" s="4"/>
+    </row>
+    <row r="465">
+      <c r="A465" s="4"/>
+    </row>
+    <row r="466">
+      <c r="A466" s="4"/>
+    </row>
+    <row r="467">
+      <c r="A467" s="4"/>
+    </row>
+    <row r="468">
+      <c r="A468" s="4"/>
+    </row>
+    <row r="469">
+      <c r="A469" s="4"/>
+    </row>
+    <row r="470">
+      <c r="A470" s="4"/>
+    </row>
+    <row r="471">
+      <c r="A471" s="4"/>
+    </row>
+    <row r="472">
+      <c r="A472" s="4"/>
+    </row>
+    <row r="473">
+      <c r="A473" s="4"/>
+    </row>
+    <row r="474">
+      <c r="A474" s="4"/>
+    </row>
+    <row r="475">
+      <c r="A475" s="4"/>
+    </row>
+    <row r="476">
+      <c r="A476" s="4"/>
+    </row>
+    <row r="477">
+      <c r="A477" s="4"/>
+    </row>
+    <row r="478">
+      <c r="A478" s="4"/>
+    </row>
+    <row r="479">
+      <c r="A479" s="4"/>
+    </row>
+    <row r="480">
+      <c r="A480" s="4"/>
+    </row>
+    <row r="481">
+      <c r="A481" s="4"/>
+    </row>
+    <row r="482">
+      <c r="A482" s="4"/>
+    </row>
+    <row r="483">
+      <c r="A483" s="4"/>
+    </row>
+    <row r="484">
+      <c r="A484" s="4"/>
+    </row>
+    <row r="485">
+      <c r="A485" s="4"/>
+    </row>
+    <row r="486">
+      <c r="A486" s="4"/>
+    </row>
+    <row r="487">
+      <c r="A487" s="4"/>
+    </row>
+    <row r="488">
+      <c r="A488" s="4"/>
+    </row>
+    <row r="489">
+      <c r="A489" s="4"/>
+    </row>
+    <row r="490">
+      <c r="A490" s="4"/>
+    </row>
+    <row r="491">
+      <c r="A491" s="4"/>
+    </row>
+    <row r="492">
+      <c r="A492" s="4"/>
+    </row>
+    <row r="493">
+      <c r="A493" s="4"/>
+    </row>
+    <row r="494">
+      <c r="A494" s="4"/>
+    </row>
+    <row r="495">
+      <c r="A495" s="4"/>
+    </row>
+    <row r="496">
+      <c r="A496" s="4"/>
+    </row>
+    <row r="497">
+      <c r="A497" s="4"/>
+    </row>
+    <row r="498">
+      <c r="A498" s="4"/>
+    </row>
+    <row r="499">
+      <c r="A499" s="4"/>
+    </row>
+    <row r="500">
+      <c r="A500" s="4"/>
+    </row>
+    <row r="501">
+      <c r="A501" s="4"/>
+    </row>
+    <row r="502">
+      <c r="A502" s="4"/>
+    </row>
+    <row r="503">
+      <c r="A503" s="4"/>
+    </row>
+    <row r="504">
+      <c r="A504" s="4"/>
+    </row>
+    <row r="505">
+      <c r="A505" s="4"/>
+    </row>
+    <row r="506">
+      <c r="A506" s="4"/>
+    </row>
+    <row r="507">
+      <c r="A507" s="4"/>
+    </row>
+    <row r="508">
+      <c r="A508" s="4"/>
+    </row>
+    <row r="509">
+      <c r="A509" s="4"/>
+    </row>
+    <row r="510">
+      <c r="A510" s="4"/>
+    </row>
+    <row r="511">
+      <c r="A511" s="4"/>
+    </row>
+    <row r="512">
+      <c r="A512" s="4"/>
+    </row>
+    <row r="513">
+      <c r="A513" s="4"/>
+    </row>
+    <row r="514">
+      <c r="A514" s="4"/>
+    </row>
+    <row r="515">
+      <c r="A515" s="4"/>
+    </row>
+    <row r="516">
+      <c r="A516" s="4"/>
+    </row>
+    <row r="517">
+      <c r="A517" s="4"/>
+    </row>
+    <row r="518">
+      <c r="A518" s="4"/>
+    </row>
+    <row r="519">
+      <c r="A519" s="4"/>
+    </row>
+    <row r="520">
+      <c r="A520" s="4"/>
+    </row>
+    <row r="521">
+      <c r="A521" s="4"/>
+    </row>
+    <row r="522">
+      <c r="A522" s="4"/>
+    </row>
+    <row r="523">
+      <c r="A523" s="4"/>
+    </row>
+    <row r="524">
+      <c r="A524" s="4"/>
+    </row>
+    <row r="525">
+      <c r="A525" s="4"/>
+    </row>
+    <row r="526">
+      <c r="A526" s="4"/>
+    </row>
+    <row r="527">
+      <c r="A527" s="4"/>
+    </row>
+    <row r="528">
+      <c r="A528" s="4"/>
+    </row>
+    <row r="529">
+      <c r="A529" s="4"/>
+    </row>
+    <row r="530">
+      <c r="A530" s="4"/>
+    </row>
+    <row r="531">
+      <c r="A531" s="4"/>
+    </row>
+    <row r="532">
+      <c r="A532" s="4"/>
+    </row>
+    <row r="533">
+      <c r="A533" s="4"/>
+    </row>
+    <row r="534">
+      <c r="A534" s="4"/>
+    </row>
+    <row r="535">
+      <c r="A535" s="4"/>
+    </row>
+    <row r="536">
+      <c r="A536" s="4"/>
+    </row>
+    <row r="537">
+      <c r="A537" s="4"/>
+    </row>
+    <row r="538">
+      <c r="A538" s="4"/>
+    </row>
+    <row r="539">
+      <c r="A539" s="4"/>
+    </row>
+    <row r="540">
+      <c r="A540" s="4"/>
+    </row>
+    <row r="541">
+      <c r="A541" s="4"/>
+    </row>
+    <row r="542">
+      <c r="A542" s="4"/>
+    </row>
+    <row r="543">
+      <c r="A543" s="4"/>
+    </row>
+    <row r="544">
+      <c r="A544" s="4"/>
+    </row>
+    <row r="545">
+      <c r="A545" s="4"/>
+    </row>
+    <row r="546">
+      <c r="A546" s="4"/>
+    </row>
+    <row r="547">
+      <c r="A547" s="4"/>
+    </row>
+    <row r="548">
+      <c r="A548" s="4"/>
+    </row>
+    <row r="549">
+      <c r="A549" s="4"/>
+    </row>
+    <row r="550">
+      <c r="A550" s="4"/>
+    </row>
+    <row r="551">
+      <c r="A551" s="4"/>
+    </row>
+    <row r="552">
+      <c r="A552" s="4"/>
+    </row>
+    <row r="553">
+      <c r="A553" s="4"/>
+    </row>
+    <row r="554">
+      <c r="A554" s="4"/>
+    </row>
+    <row r="555">
+      <c r="A555" s="4"/>
+    </row>
+    <row r="556">
+      <c r="A556" s="4"/>
+    </row>
+    <row r="557">
+      <c r="A557" s="4"/>
+    </row>
+    <row r="558">
+      <c r="A558" s="4"/>
+    </row>
+    <row r="559">
+      <c r="A559" s="4"/>
+    </row>
+    <row r="560">
+      <c r="A560" s="4"/>
+    </row>
+    <row r="561">
+      <c r="A561" s="4"/>
+    </row>
+    <row r="562">
+      <c r="A562" s="4"/>
+    </row>
+    <row r="563">
+      <c r="A563" s="4"/>
+    </row>
+    <row r="564">
+      <c r="A564" s="4"/>
+    </row>
+    <row r="565">
+      <c r="A565" s="4"/>
+    </row>
+    <row r="566">
+      <c r="A566" s="4"/>
+    </row>
+    <row r="567">
+      <c r="A567" s="4"/>
+    </row>
+    <row r="568">
+      <c r="A568" s="4"/>
+    </row>
+    <row r="569">
+      <c r="A569" s="4"/>
+    </row>
+    <row r="570">
+      <c r="A570" s="4"/>
+    </row>
+    <row r="571">
+      <c r="A571" s="4"/>
+    </row>
+    <row r="572">
+      <c r="A572" s="4"/>
+    </row>
+    <row r="573">
+      <c r="A573" s="4"/>
+    </row>
+    <row r="574">
+      <c r="A574" s="4"/>
+    </row>
+    <row r="575">
+      <c r="A575" s="4"/>
+    </row>
+    <row r="576">
+      <c r="A576" s="4"/>
+    </row>
+    <row r="577">
+      <c r="A577" s="4"/>
+    </row>
+    <row r="578">
+      <c r="A578" s="4"/>
+    </row>
+    <row r="579">
+      <c r="A579" s="4"/>
+    </row>
+    <row r="580">
+      <c r="A580" s="4"/>
+    </row>
+    <row r="581">
+      <c r="A581" s="4"/>
+    </row>
+    <row r="582">
+      <c r="A582" s="4"/>
+    </row>
+    <row r="583">
+      <c r="A583" s="4"/>
+    </row>
+    <row r="584">
+      <c r="A584" s="4"/>
+    </row>
+    <row r="585">
+      <c r="A585" s="4"/>
+    </row>
+    <row r="586">
+      <c r="A586" s="4"/>
+    </row>
+    <row r="587">
+      <c r="A587" s="4"/>
+    </row>
+    <row r="588">
+      <c r="A588" s="4"/>
+    </row>
+    <row r="589">
+      <c r="A589" s="4"/>
+    </row>
+    <row r="590">
+      <c r="A590" s="4"/>
+    </row>
+    <row r="591">
+      <c r="A591" s="4"/>
+    </row>
+    <row r="592">
+      <c r="A592" s="4"/>
+    </row>
+    <row r="593">
+      <c r="A593" s="4"/>
+    </row>
+    <row r="594">
+      <c r="A594" s="4"/>
+    </row>
+    <row r="595">
+      <c r="A595" s="4"/>
+    </row>
+    <row r="596">
+      <c r="A596" s="4"/>
+    </row>
+    <row r="597">
+      <c r="A597" s="4"/>
+    </row>
+    <row r="598">
+      <c r="A598" s="4"/>
+    </row>
+    <row r="599">
+      <c r="A599" s="4"/>
+    </row>
+    <row r="600">
+      <c r="A600" s="4"/>
+    </row>
+    <row r="601">
+      <c r="A601" s="4"/>
+    </row>
+    <row r="602">
+      <c r="A602" s="4"/>
+    </row>
+    <row r="603">
+      <c r="A603" s="4"/>
+    </row>
+    <row r="604">
+      <c r="A604" s="4"/>
+    </row>
+    <row r="605">
+      <c r="A605" s="4"/>
+    </row>
+    <row r="606">
+      <c r="A606" s="4"/>
+    </row>
+    <row r="607">
+      <c r="A607" s="4"/>
+    </row>
+    <row r="608">
+      <c r="A608" s="4"/>
+    </row>
+    <row r="609">
+      <c r="A609" s="4"/>
+    </row>
+    <row r="610">
+      <c r="A610" s="4"/>
+    </row>
+    <row r="611">
+      <c r="A611" s="4"/>
+    </row>
+    <row r="612">
+      <c r="A612" s="4"/>
+    </row>
+    <row r="613">
+      <c r="A613" s="4"/>
+    </row>
+    <row r="614">
+      <c r="A614" s="4"/>
+    </row>
+    <row r="615">
+      <c r="A615" s="4"/>
+    </row>
+    <row r="616">
+      <c r="A616" s="4"/>
+    </row>
+    <row r="617">
+      <c r="A617" s="4"/>
+    </row>
+    <row r="618">
+      <c r="A618" s="4"/>
+    </row>
+    <row r="619">
+      <c r="A619" s="4"/>
+    </row>
+    <row r="620">
+      <c r="A620" s="4"/>
+    </row>
+    <row r="621">
+      <c r="A621" s="4"/>
+    </row>
+    <row r="622">
+      <c r="A622" s="4"/>
+    </row>
+    <row r="623">
+      <c r="A623" s="4"/>
+    </row>
+    <row r="624">
+      <c r="A624" s="4"/>
+    </row>
+    <row r="625">
+      <c r="A625" s="4"/>
+    </row>
+    <row r="626">
+      <c r="A626" s="4"/>
+    </row>
+    <row r="627">
+      <c r="A627" s="4"/>
+    </row>
+    <row r="628">
+      <c r="A628" s="4"/>
+    </row>
+    <row r="629">
+      <c r="A629" s="4"/>
+    </row>
+    <row r="630">
+      <c r="A630" s="4"/>
+    </row>
+    <row r="631">
+      <c r="A631" s="4"/>
+    </row>
+    <row r="632">
+      <c r="A632" s="4"/>
+    </row>
+    <row r="633">
+      <c r="A633" s="4"/>
+    </row>
+    <row r="634">
+      <c r="A634" s="4"/>
+    </row>
+    <row r="635">
+      <c r="A635" s="4"/>
+    </row>
+    <row r="636">
+      <c r="A636" s="4"/>
+    </row>
+    <row r="637">
+      <c r="A637" s="4"/>
+    </row>
+    <row r="638">
+      <c r="A638" s="4"/>
+    </row>
+    <row r="639">
+      <c r="A639" s="4"/>
+    </row>
+    <row r="640">
+      <c r="A640" s="4"/>
+    </row>
+    <row r="641">
+      <c r="A641" s="4"/>
+    </row>
+    <row r="642">
+      <c r="A642" s="4"/>
+    </row>
+    <row r="643">
+      <c r="A643" s="4"/>
+    </row>
+    <row r="644">
+      <c r="A644" s="4"/>
+    </row>
+    <row r="645">
+      <c r="A645" s="4"/>
+    </row>
+    <row r="646">
+      <c r="A646" s="4"/>
+    </row>
+    <row r="647">
+      <c r="A647" s="4"/>
+    </row>
+    <row r="648">
+      <c r="A648" s="4"/>
+    </row>
+    <row r="649">
+      <c r="A649" s="4"/>
+    </row>
+    <row r="650">
+      <c r="A650" s="4"/>
+    </row>
+    <row r="651">
+      <c r="A651" s="4"/>
+    </row>
+    <row r="652">
+      <c r="A652" s="4"/>
+    </row>
+    <row r="653">
+      <c r="A653" s="4"/>
+    </row>
+    <row r="654">
+      <c r="A654" s="4"/>
+    </row>
+    <row r="655">
+      <c r="A655" s="4"/>
+    </row>
+    <row r="656">
+      <c r="A656" s="4"/>
+    </row>
+    <row r="657">
+      <c r="A657" s="4"/>
+    </row>
+    <row r="658">
+      <c r="A658" s="4"/>
+    </row>
+    <row r="659">
+      <c r="A659" s="4"/>
+    </row>
+    <row r="660">
+      <c r="A660" s="4"/>
+    </row>
+    <row r="661">
+      <c r="A661" s="4"/>
+    </row>
+    <row r="662">
+      <c r="A662" s="4"/>
+    </row>
+    <row r="663">
+      <c r="A663" s="4"/>
+    </row>
+    <row r="664">
+      <c r="A664" s="4"/>
+    </row>
+    <row r="665">
+      <c r="A665" s="4"/>
+    </row>
+    <row r="666">
+      <c r="A666" s="4"/>
+    </row>
+    <row r="667">
+      <c r="A667" s="4"/>
+    </row>
+    <row r="668">
+      <c r="A668" s="4"/>
+    </row>
+    <row r="669">
+      <c r="A669" s="4"/>
+    </row>
+    <row r="670">
+      <c r="A670" s="4"/>
+    </row>
+    <row r="671">
+      <c r="A671" s="4"/>
+    </row>
+    <row r="672">
+      <c r="A672" s="4"/>
+    </row>
+    <row r="673">
+      <c r="A673" s="4"/>
+    </row>
+    <row r="674">
+      <c r="A674" s="4"/>
+    </row>
+    <row r="675">
+      <c r="A675" s="4"/>
+    </row>
+    <row r="676">
+      <c r="A676" s="4"/>
+    </row>
+    <row r="677">
+      <c r="A677" s="4"/>
+    </row>
+    <row r="678">
+      <c r="A678" s="4"/>
+    </row>
+    <row r="679">
+      <c r="A679" s="4"/>
+    </row>
+    <row r="680">
+      <c r="A680" s="4"/>
+    </row>
+    <row r="681">
+      <c r="A681" s="4"/>
+    </row>
+    <row r="682">
+      <c r="A682" s="4"/>
+    </row>
+    <row r="683">
+      <c r="A683" s="4"/>
+    </row>
+    <row r="684">
+      <c r="A684" s="4"/>
+    </row>
+    <row r="685">
+      <c r="A685" s="4"/>
+    </row>
+    <row r="686">
+      <c r="A686" s="4"/>
+    </row>
+    <row r="687">
+      <c r="A687" s="4"/>
+    </row>
+    <row r="688">
+      <c r="A688" s="4"/>
+    </row>
+    <row r="689">
+      <c r="A689" s="4"/>
+    </row>
+    <row r="690">
+      <c r="A690" s="4"/>
+    </row>
+    <row r="691">
+      <c r="A691" s="4"/>
+    </row>
+    <row r="692">
+      <c r="A692" s="4"/>
+    </row>
+    <row r="693">
+      <c r="A693" s="4"/>
+    </row>
+    <row r="694">
+      <c r="A694" s="4"/>
+    </row>
+    <row r="695">
+      <c r="A695" s="4"/>
+    </row>
+    <row r="696">
+      <c r="A696" s="4"/>
+    </row>
+    <row r="697">
+      <c r="A697" s="4"/>
+    </row>
+    <row r="698">
+      <c r="A698" s="4"/>
+    </row>
+    <row r="699">
+      <c r="A699" s="4"/>
+    </row>
+    <row r="700">
+      <c r="A700" s="4"/>
+    </row>
+    <row r="701">
+      <c r="A701" s="4"/>
+    </row>
+    <row r="702">
+      <c r="A702" s="4"/>
+    </row>
+    <row r="703">
+      <c r="A703" s="4"/>
+    </row>
+    <row r="704">
+      <c r="A704" s="4"/>
+    </row>
+    <row r="705">
+      <c r="A705" s="4"/>
+    </row>
+    <row r="706">
+      <c r="A706" s="4"/>
+    </row>
+    <row r="707">
+      <c r="A707" s="4"/>
+    </row>
+    <row r="708">
+      <c r="A708" s="4"/>
+    </row>
+    <row r="709">
+      <c r="A709" s="4"/>
+    </row>
+    <row r="710">
+      <c r="A710" s="4"/>
+    </row>
+    <row r="711">
+      <c r="A711" s="4"/>
+    </row>
+    <row r="712">
+      <c r="A712" s="4"/>
+    </row>
+    <row r="713">
+      <c r="A713" s="4"/>
+    </row>
+    <row r="714">
+      <c r="A714" s="4"/>
+    </row>
+    <row r="715">
+      <c r="A715" s="4"/>
+    </row>
+    <row r="716">
+      <c r="A716" s="4"/>
+    </row>
+    <row r="717">
+      <c r="A717" s="4"/>
+    </row>
+    <row r="718">
+      <c r="A718" s="4"/>
+    </row>
+    <row r="719">
+      <c r="A719" s="4"/>
+    </row>
+    <row r="720">
+      <c r="A720" s="4"/>
+    </row>
+    <row r="721">
+      <c r="A721" s="4"/>
+    </row>
+    <row r="722">
+      <c r="A722" s="4"/>
+    </row>
+    <row r="723">
+      <c r="A723" s="4"/>
+    </row>
+    <row r="724">
+      <c r="A724" s="4"/>
+    </row>
+    <row r="725">
+      <c r="A725" s="4"/>
+    </row>
+    <row r="726">
+      <c r="A726" s="4"/>
+    </row>
+    <row r="727">
+      <c r="A727" s="4"/>
+    </row>
+    <row r="728">
+      <c r="A728" s="4"/>
+    </row>
+    <row r="729">
+      <c r="A729" s="4"/>
+    </row>
+    <row r="730">
+      <c r="A730" s="4"/>
+    </row>
+    <row r="731">
+      <c r="A731" s="4"/>
+    </row>
+    <row r="732">
+      <c r="A732" s="4"/>
+    </row>
+    <row r="733">
+      <c r="A733" s="4"/>
+    </row>
+    <row r="734">
+      <c r="A734" s="4"/>
+    </row>
+    <row r="735">
+      <c r="A735" s="4"/>
+    </row>
+    <row r="736">
+      <c r="A736" s="4"/>
+    </row>
+    <row r="737">
+      <c r="A737" s="4"/>
+    </row>
+    <row r="738">
+      <c r="A738" s="4"/>
+    </row>
+    <row r="739">
+      <c r="A739" s="4"/>
+    </row>
+    <row r="740">
+      <c r="A740" s="4"/>
+    </row>
+    <row r="741">
+      <c r="A741" s="4"/>
+    </row>
+    <row r="742">
+      <c r="A742" s="4"/>
+    </row>
+    <row r="743">
+      <c r="A743" s="4"/>
+    </row>
+    <row r="744">
+      <c r="A744" s="4"/>
+    </row>
+    <row r="745">
+      <c r="A745" s="4"/>
+    </row>
+    <row r="746">
+      <c r="A746" s="4"/>
+    </row>
+    <row r="747">
+      <c r="A747" s="4"/>
+    </row>
+    <row r="748">
+      <c r="A748" s="4"/>
+    </row>
+    <row r="749">
+      <c r="A749" s="4"/>
+    </row>
+    <row r="750">
+      <c r="A750" s="4"/>
+    </row>
+    <row r="751">
+      <c r="A751" s="4"/>
+    </row>
+    <row r="752">
+      <c r="A752" s="4"/>
+    </row>
+    <row r="753">
+      <c r="A753" s="4"/>
+    </row>
+    <row r="754">
+      <c r="A754" s="4"/>
+    </row>
+    <row r="755">
+      <c r="A755" s="4"/>
+    </row>
+    <row r="756">
+      <c r="A756" s="4"/>
+    </row>
+    <row r="757">
+      <c r="A757" s="4"/>
+    </row>
+    <row r="758">
+      <c r="A758" s="4"/>
+    </row>
+    <row r="759">
+      <c r="A759" s="4"/>
+    </row>
+    <row r="760">
+      <c r="A760" s="4"/>
+    </row>
+    <row r="761">
+      <c r="A761" s="4"/>
+    </row>
+    <row r="762">
+      <c r="A762" s="4"/>
+    </row>
+    <row r="763">
+      <c r="A763" s="4"/>
+    </row>
+    <row r="764">
+      <c r="A764" s="4"/>
+    </row>
+    <row r="765">
+      <c r="A765" s="4"/>
+    </row>
+    <row r="766">
+      <c r="A766" s="4"/>
+    </row>
+    <row r="767">
+      <c r="A767" s="4"/>
+    </row>
+    <row r="768">
+      <c r="A768" s="4"/>
+    </row>
+    <row r="769">
+      <c r="A769" s="4"/>
+    </row>
+    <row r="770">
+      <c r="A770" s="4"/>
+    </row>
+    <row r="771">
+      <c r="A771" s="4"/>
+    </row>
+    <row r="772">
+      <c r="A772" s="4"/>
+    </row>
+    <row r="773">
+      <c r="A773" s="4"/>
+    </row>
+    <row r="774">
+      <c r="A774" s="4"/>
+    </row>
+    <row r="775">
+      <c r="A775" s="4"/>
+    </row>
+    <row r="776">
+      <c r="A776" s="4"/>
+    </row>
+    <row r="777">
+      <c r="A777" s="4"/>
+    </row>
+    <row r="778">
+      <c r="A778" s="4"/>
+    </row>
+    <row r="779">
+      <c r="A779" s="4"/>
+    </row>
+    <row r="780">
+      <c r="A780" s="4"/>
+    </row>
+    <row r="781">
+      <c r="A781" s="4"/>
+    </row>
+    <row r="782">
+      <c r="A782" s="4"/>
+    </row>
+    <row r="783">
+      <c r="A783" s="4"/>
+    </row>
+    <row r="784">
+      <c r="A784" s="4"/>
+    </row>
+    <row r="785">
+      <c r="A785" s="4"/>
+    </row>
+    <row r="786">
+      <c r="A786" s="4"/>
+    </row>
+    <row r="787">
+      <c r="A787" s="4"/>
+    </row>
+    <row r="788">
+      <c r="A788" s="4"/>
+    </row>
+    <row r="789">
+      <c r="A789" s="4"/>
+    </row>
+    <row r="790">
+      <c r="A790" s="4"/>
+    </row>
+    <row r="791">
+      <c r="A791" s="4"/>
+    </row>
+    <row r="792">
+      <c r="A792" s="4"/>
+    </row>
+    <row r="793">
+      <c r="A793" s="4"/>
+    </row>
+    <row r="794">
+      <c r="A794" s="4"/>
+    </row>
+    <row r="795">
+      <c r="A795" s="4"/>
+    </row>
+    <row r="796">
+      <c r="A796" s="4"/>
+    </row>
+    <row r="797">
+      <c r="A797" s="4"/>
+    </row>
+    <row r="798">
+      <c r="A798" s="4"/>
+    </row>
+    <row r="799">
+      <c r="A799" s="4"/>
+    </row>
+    <row r="800">
+      <c r="A800" s="4"/>
+    </row>
+    <row r="801">
+      <c r="A801" s="4"/>
+    </row>
+    <row r="802">
+      <c r="A802" s="4"/>
+    </row>
+    <row r="803">
+      <c r="A803" s="4"/>
+    </row>
+    <row r="804">
+      <c r="A804" s="4"/>
+    </row>
+    <row r="805">
+      <c r="A805" s="4"/>
+    </row>
+    <row r="806">
+      <c r="A806" s="4"/>
+    </row>
+    <row r="807">
+      <c r="A807" s="4"/>
+    </row>
+    <row r="808">
+      <c r="A808" s="4"/>
+    </row>
+    <row r="809">
+      <c r="A809" s="4"/>
+    </row>
+    <row r="810">
+      <c r="A810" s="4"/>
+    </row>
+    <row r="811">
+      <c r="A811" s="4"/>
+    </row>
+    <row r="812">
+      <c r="A812" s="4"/>
+    </row>
+    <row r="813">
+      <c r="A813" s="4"/>
+    </row>
+    <row r="814">
+      <c r="A814" s="4"/>
+    </row>
+    <row r="815">
+      <c r="A815" s="4"/>
+    </row>
+    <row r="816">
+      <c r="A816" s="4"/>
+    </row>
+    <row r="817">
+      <c r="A817" s="4"/>
+    </row>
+    <row r="818">
+      <c r="A818" s="4"/>
+    </row>
+    <row r="819">
+      <c r="A819" s="4"/>
+    </row>
+    <row r="820">
+      <c r="A820" s="4"/>
+    </row>
+    <row r="821">
+      <c r="A821" s="4"/>
+    </row>
+    <row r="822">
+      <c r="A822" s="4"/>
+    </row>
+    <row r="823">
+      <c r="A823" s="4"/>
+    </row>
+    <row r="824">
+      <c r="A824" s="4"/>
+    </row>
+    <row r="825">
+      <c r="A825" s="4"/>
+    </row>
+    <row r="826">
+      <c r="A826" s="4"/>
+    </row>
+    <row r="827">
+      <c r="A827" s="4"/>
+    </row>
+    <row r="828">
+      <c r="A828" s="4"/>
+    </row>
+    <row r="829">
+      <c r="A829" s="4"/>
+    </row>
+    <row r="830">
+      <c r="A830" s="4"/>
+    </row>
+    <row r="831">
+      <c r="A831" s="4"/>
+    </row>
+    <row r="832">
+      <c r="A832" s="4"/>
+    </row>
+    <row r="833">
+      <c r="A833" s="4"/>
+    </row>
+    <row r="834">
+      <c r="A834" s="4"/>
+    </row>
+    <row r="835">
+      <c r="A835" s="4"/>
+    </row>
+    <row r="836">
+      <c r="A836" s="4"/>
+    </row>
+    <row r="837">
+      <c r="A837" s="4"/>
+    </row>
+    <row r="838">
+      <c r="A838" s="4"/>
+    </row>
+    <row r="839">
+      <c r="A839" s="4"/>
+    </row>
+    <row r="840">
+      <c r="A840" s="4"/>
+    </row>
+    <row r="841">
+      <c r="A841" s="4"/>
+    </row>
+    <row r="842">
+      <c r="A842" s="4"/>
+    </row>
+    <row r="843">
+      <c r="A843" s="4"/>
+    </row>
+    <row r="844">
+      <c r="A844" s="4"/>
+    </row>
+    <row r="845">
+      <c r="A845" s="4"/>
+    </row>
+    <row r="846">
+      <c r="A846" s="4"/>
+    </row>
+    <row r="847">
+      <c r="A847" s="4"/>
+    </row>
+    <row r="848">
+      <c r="A848" s="4"/>
+    </row>
+    <row r="849">
+      <c r="A849" s="4"/>
+    </row>
+    <row r="850">
+      <c r="A850" s="4"/>
+    </row>
+    <row r="851">
+      <c r="A851" s="4"/>
+    </row>
+    <row r="852">
+      <c r="A852" s="4"/>
+    </row>
+    <row r="853">
+      <c r="A853" s="4"/>
+    </row>
+    <row r="854">
+      <c r="A854" s="4"/>
+    </row>
+    <row r="855">
+      <c r="A855" s="4"/>
+    </row>
+    <row r="856">
+      <c r="A856" s="4"/>
+    </row>
+    <row r="857">
+      <c r="A857" s="4"/>
+    </row>
+    <row r="858">
+      <c r="A858" s="4"/>
+    </row>
+    <row r="859">
+      <c r="A859" s="4"/>
+    </row>
+    <row r="860">
+      <c r="A860" s="4"/>
+    </row>
+    <row r="861">
+      <c r="A861" s="4"/>
+    </row>
+    <row r="862">
+      <c r="A862" s="4"/>
+    </row>
+    <row r="863">
+      <c r="A863" s="4"/>
+    </row>
+    <row r="864">
+      <c r="A864" s="4"/>
+    </row>
+    <row r="865">
+      <c r="A865" s="4"/>
+    </row>
+    <row r="866">
+      <c r="A866" s="4"/>
+    </row>
+    <row r="867">
+      <c r="A867" s="4"/>
+    </row>
+    <row r="868">
+      <c r="A868" s="4"/>
+    </row>
+    <row r="869">
+      <c r="A869" s="4"/>
+    </row>
+    <row r="870">
+      <c r="A870" s="4"/>
+    </row>
+    <row r="871">
+      <c r="A871" s="4"/>
+    </row>
+    <row r="872">
+      <c r="A872" s="4"/>
+    </row>
+    <row r="873">
+      <c r="A873" s="4"/>
+    </row>
+    <row r="874">
+      <c r="A874" s="4"/>
+    </row>
+    <row r="875">
+      <c r="A875" s="4"/>
+    </row>
+    <row r="876">
+      <c r="A876" s="4"/>
+    </row>
+    <row r="877">
+      <c r="A877" s="4"/>
+    </row>
+    <row r="878">
+      <c r="A878" s="4"/>
+    </row>
+    <row r="879">
+      <c r="A879" s="4"/>
+    </row>
+    <row r="880">
+      <c r="A880" s="4"/>
+    </row>
+    <row r="881">
+      <c r="A881" s="4"/>
+    </row>
+    <row r="882">
+      <c r="A882" s="4"/>
+    </row>
+    <row r="883">
+      <c r="A883" s="4"/>
+    </row>
+    <row r="884">
+      <c r="A884" s="4"/>
+    </row>
+    <row r="885">
+      <c r="A885" s="4"/>
+    </row>
+    <row r="886">
+      <c r="A886" s="4"/>
+    </row>
+    <row r="887">
+      <c r="A887" s="4"/>
+    </row>
+    <row r="888">
+      <c r="A888" s="4"/>
+    </row>
+    <row r="889">
+      <c r="A889" s="4"/>
+    </row>
+    <row r="890">
+      <c r="A890" s="4"/>
+    </row>
+    <row r="891">
+      <c r="A891" s="4"/>
+    </row>
+    <row r="892">
+      <c r="A892" s="4"/>
+    </row>
+    <row r="893">
+      <c r="A893" s="4"/>
+    </row>
+    <row r="894">
+      <c r="A894" s="4"/>
+    </row>
+    <row r="895">
+      <c r="A895" s="4"/>
+    </row>
+    <row r="896">
+      <c r="A896" s="4"/>
+    </row>
+    <row r="897">
+      <c r="A897" s="4"/>
+    </row>
+    <row r="898">
+      <c r="A898" s="4"/>
+    </row>
+    <row r="899">
+      <c r="A899" s="4"/>
+    </row>
+    <row r="900">
+      <c r="A900" s="4"/>
+    </row>
+    <row r="901">
+      <c r="A901" s="4"/>
+    </row>
+    <row r="902">
+      <c r="A902" s="4"/>
+    </row>
+    <row r="903">
+      <c r="A903" s="4"/>
+    </row>
+    <row r="904">
+      <c r="A904" s="4"/>
+    </row>
+    <row r="905">
+      <c r="A905" s="4"/>
+    </row>
+    <row r="906">
+      <c r="A906" s="4"/>
+    </row>
+    <row r="907">
+      <c r="A907" s="4"/>
+    </row>
+    <row r="908">
+      <c r="A908" s="4"/>
+    </row>
+    <row r="909">
+      <c r="A909" s="4"/>
+    </row>
+    <row r="910">
+      <c r="A910" s="4"/>
+    </row>
+    <row r="911">
+      <c r="A911" s="4"/>
+    </row>
+    <row r="912">
+      <c r="A912" s="4"/>
+    </row>
+    <row r="913">
+      <c r="A913" s="4"/>
+    </row>
+    <row r="914">
+      <c r="A914" s="4"/>
+    </row>
+    <row r="915">
+      <c r="A915" s="4"/>
+    </row>
+    <row r="916">
+      <c r="A916" s="4"/>
+    </row>
+    <row r="917">
+      <c r="A917" s="4"/>
+    </row>
+    <row r="918">
+      <c r="A918" s="4"/>
+    </row>
+    <row r="919">
+      <c r="A919" s="4"/>
+    </row>
+    <row r="920">
+      <c r="A920" s="4"/>
+    </row>
+    <row r="921">
+      <c r="A921" s="4"/>
+    </row>
+    <row r="922">
+      <c r="A922" s="4"/>
+    </row>
+    <row r="923">
+      <c r="A923" s="4"/>
+    </row>
+    <row r="924">
+      <c r="A924" s="4"/>
+    </row>
+    <row r="925">
+      <c r="A925" s="4"/>
+    </row>
+    <row r="926">
+      <c r="A926" s="4"/>
+    </row>
+    <row r="927">
+      <c r="A927" s="4"/>
+    </row>
+    <row r="928">
+      <c r="A928" s="4"/>
+    </row>
+    <row r="929">
+      <c r="A929" s="4"/>
+    </row>
+    <row r="930">
+      <c r="A930" s="4"/>
+    </row>
+    <row r="931">
+      <c r="A931" s="4"/>
+    </row>
+    <row r="932">
+      <c r="A932" s="4"/>
+    </row>
+    <row r="933">
+      <c r="A933" s="4"/>
+    </row>
+    <row r="934">
+      <c r="A934" s="4"/>
+    </row>
+    <row r="935">
+      <c r="A935" s="4"/>
+    </row>
+    <row r="936">
+      <c r="A936" s="4"/>
+    </row>
+    <row r="937">
+      <c r="A937" s="4"/>
+    </row>
+    <row r="938">
+      <c r="A938" s="4"/>
+    </row>
+    <row r="939">
+      <c r="A939" s="4"/>
+    </row>
+    <row r="940">
+      <c r="A940" s="4"/>
+    </row>
+    <row r="941">
+      <c r="A941" s="4"/>
+    </row>
+    <row r="942">
+      <c r="A942" s="4"/>
+    </row>
+    <row r="943">
+      <c r="A943" s="4"/>
+    </row>
+    <row r="944">
+      <c r="A944" s="4"/>
+    </row>
+    <row r="945">
+      <c r="A945" s="4"/>
+    </row>
+    <row r="946">
+      <c r="A946" s="4"/>
+    </row>
+    <row r="947">
+      <c r="A947" s="4"/>
+    </row>
+    <row r="948">
+      <c r="A948" s="4"/>
+    </row>
+    <row r="949">
+      <c r="A949" s="4"/>
+    </row>
+    <row r="950">
+      <c r="A950" s="4"/>
+    </row>
+    <row r="951">
+      <c r="A951" s="4"/>
+    </row>
+    <row r="952">
+      <c r="A952" s="4"/>
+    </row>
+    <row r="953">
+      <c r="A953" s="4"/>
+    </row>
+    <row r="954">
+      <c r="A954" s="4"/>
+    </row>
+    <row r="955">
+      <c r="A955" s="4"/>
+    </row>
+    <row r="956">
+      <c r="A956" s="4"/>
+    </row>
+    <row r="957">
+      <c r="A957" s="4"/>
+    </row>
+    <row r="958">
+      <c r="A958" s="4"/>
+    </row>
+    <row r="959">
+      <c r="A959" s="4"/>
+    </row>
+    <row r="960">
+      <c r="A960" s="4"/>
+    </row>
+    <row r="961">
+      <c r="A961" s="4"/>
+    </row>
+    <row r="962">
+      <c r="A962" s="4"/>
+    </row>
+    <row r="963">
+      <c r="A963" s="4"/>
+    </row>
+    <row r="964">
+      <c r="A964" s="4"/>
+    </row>
+    <row r="965">
+      <c r="A965" s="4"/>
+    </row>
+    <row r="966">
+      <c r="A966" s="4"/>
+    </row>
+    <row r="967">
+      <c r="A967" s="4"/>
+    </row>
+    <row r="968">
+      <c r="A968" s="4"/>
+    </row>
+    <row r="969">
+      <c r="A969" s="4"/>
+    </row>
+    <row r="970">
+      <c r="A970" s="4"/>
+    </row>
+    <row r="971">
+      <c r="A971" s="4"/>
+    </row>
+    <row r="972">
+      <c r="A972" s="4"/>
+    </row>
+    <row r="973">
+      <c r="A973" s="4"/>
+    </row>
+    <row r="974">
+      <c r="A974" s="4"/>
+    </row>
+    <row r="975">
+      <c r="A975" s="4"/>
+    </row>
+    <row r="976">
+      <c r="A976" s="4"/>
+    </row>
+    <row r="977">
+      <c r="A977" s="4"/>
+    </row>
+    <row r="978">
+      <c r="A978" s="4"/>
+    </row>
+    <row r="979">
+      <c r="A979" s="4"/>
+    </row>
+    <row r="980">
+      <c r="A980" s="4"/>
+    </row>
+    <row r="981">
+      <c r="A981" s="4"/>
+    </row>
+    <row r="982">
+      <c r="A982" s="4"/>
+    </row>
+    <row r="983">
+      <c r="A983" s="4"/>
+    </row>
+    <row r="984">
+      <c r="A984" s="4"/>
+    </row>
+    <row r="985">
+      <c r="A985" s="4"/>
+    </row>
+    <row r="986">
+      <c r="A986" s="4"/>
+    </row>
+    <row r="987">
+      <c r="A987" s="4"/>
+    </row>
+    <row r="988">
+      <c r="A988" s="4"/>
+    </row>
+    <row r="989">
+      <c r="A989" s="4"/>
+    </row>
+    <row r="990">
+      <c r="A990" s="4"/>
+    </row>
+    <row r="991">
+      <c r="A991" s="4"/>
+    </row>
+    <row r="992">
+      <c r="A992" s="4"/>
+    </row>
+    <row r="993">
+      <c r="A993" s="4"/>
+    </row>
+    <row r="994">
+      <c r="A994" s="4"/>
+    </row>
+    <row r="995">
+      <c r="A995" s="4"/>
+    </row>
+    <row r="996">
+      <c r="A996" s="4"/>
+    </row>
+    <row r="997">
+      <c r="A997" s="4"/>
+    </row>
+    <row r="998">
+      <c r="A998" s="4"/>
+    </row>
+    <row r="999">
+      <c r="A999" s="4"/>
+    </row>
+    <row r="1000">
+      <c r="A1000" s="4"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>